<commit_message>
Updated the Project Rubric
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="80">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -436,6 +436,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>II</t>
   </si>
 </sst>
 </file>
@@ -959,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1092,7 +1095,7 @@
       </c>
       <c r="I4" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="J4" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
@@ -1100,11 +1103,11 @@
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>29</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1165,7 +1168,7 @@
       </c>
       <c r="H6" s="5">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91)  &gt; 22, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) - 22,0)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I6" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 22,0)</f>
@@ -1237,11 +1240,11 @@
       </c>
       <c r="I8" s="9">
         <f>I4+IF(I4 &lt; 22, IF(H10+I4 &gt; 22, 22- I4, H10),0)</f>
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="J8" s="9">
         <f>J4+IF(J4 &lt; 22, IF(I10+J4 &gt; 22, 22- J4, I10),0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1298,11 +1301,11 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
@@ -1507,11 +1510,15 @@
       <c r="D20" s="5">
         <v>5</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="3"/>
+      <c r="E20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G20" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -1752,11 +1759,15 @@
       <c r="D31" s="5">
         <v>3</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="3"/>
+      <c r="E31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G31" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -1777,11 +1788,15 @@
       <c r="D32" s="5">
         <v>3</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="3"/>
+      <c r="E32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G32" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
@@ -1802,11 +1817,15 @@
       <c r="D33" s="5">
         <v>1</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="3"/>
+      <c r="E33" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G33" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
@@ -1827,11 +1846,15 @@
       <c r="D34" s="5">
         <v>1</v>
       </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="3"/>
+      <c r="E34" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G34" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
@@ -1852,11 +1875,15 @@
       <c r="D35" s="5">
         <v>1</v>
       </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="3"/>
+      <c r="E35" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G35" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
@@ -1877,11 +1904,15 @@
       <c r="D36" s="5">
         <v>2</v>
       </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="3"/>
+      <c r="E36" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G36" s="8">
         <f t="shared" ref="G36:G67" si="1" xml:space="preserve"> IF(EXACT(F36,"X"),IF(EXACT(E36,"I"),$B36,IF(EXACT(E36,"II"),$C36,IF(EXACT(E36,"III"),$D36,0))),0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
@@ -2939,7 +2970,9 @@
       <c r="B90" s="6">
         <v>3</v>
       </c>
-      <c r="C90" s="3"/>
+      <c r="C90" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
       <c r="F90" s="5"/>
@@ -2957,7 +2990,9 @@
       <c r="B91" s="6">
         <v>1</v>
       </c>
-      <c r="C91" s="3"/>
+      <c r="C91" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
       <c r="F91" s="5"/>
@@ -3092,7 +3127,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added Transparency Objects into the scene with proper sorting
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="81">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -439,6 +439,9 @@
   </si>
   <si>
     <t>II</t>
+  </si>
+  <si>
+    <t>III</t>
   </si>
 </sst>
 </file>
@@ -962,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1095,19 +1098,19 @@
       </c>
       <c r="I4" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="J4" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>52</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1172,7 +1175,7 @@
       </c>
       <c r="I6" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 22,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) - 22,0)</f>
@@ -1181,7 +1184,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="9">
         <f>IF(L4 &gt; 66, SUM(-66,L4),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -1244,7 +1247,7 @@
       </c>
       <c r="J8" s="9">
         <f>J4+IF(J4 &lt; 22, IF(I10+J4 &gt; 22, 22- J4, I10),0)</f>
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1301,15 +1304,15 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1618,11 +1621,15 @@
       <c r="D24" s="5">
         <v>5</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="3"/>
+      <c r="E24" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G24" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -2586,11 +2593,15 @@
       <c r="D68" s="5">
         <v>5</v>
       </c>
-      <c r="E68" s="2"/>
-      <c r="F68" s="3"/>
+      <c r="E68" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G68" s="8">
         <f t="shared" ref="G68:G85" si="2" xml:space="preserve"> IF(EXACT(F68,"X"),IF(EXACT(E68,"I"),$B68,IF(EXACT(E68,"II"),$C68,IF(EXACT(E68,"III"),$D68,0))),0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
@@ -2973,8 +2984,12 @@
       <c r="C90" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D90" s="3"/>
-      <c r="E90" s="3"/>
+      <c r="D90" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
@@ -2993,8 +3008,12 @@
       <c r="C91" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D91" s="3"/>
-      <c r="E91" s="3"/>
+      <c r="D91" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
       <c r="H91" s="5"/>
@@ -3127,7 +3146,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Fixed resizing of the window, started on adding multiple viewports
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="81">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -965,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="J4" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
@@ -1110,7 +1110,7 @@
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1184,7 +1184,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="9">
         <f>IF(L4 &gt; 66, SUM(-66,L4),0)</f>
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -1312,7 +1312,7 @@
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -2314,11 +2314,15 @@
       <c r="D55" s="5">
         <v>3</v>
       </c>
-      <c r="E55" s="2"/>
-      <c r="F55" s="3"/>
+      <c r="E55" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G55" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
@@ -2339,11 +2343,15 @@
       <c r="D56" s="5">
         <v>5</v>
       </c>
-      <c r="E56" s="2"/>
-      <c r="F56" s="3"/>
+      <c r="E56" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G56" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
@@ -3146,7 +3154,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Finished implementing a second viewport for a minimap
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="81">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -965,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1106,11 +1106,11 @@
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1179,12 +1179,12 @@
       </c>
       <c r="J6" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) - 22,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="9">
         <f>IF(L4 &gt; 66, SUM(-66,L4),0)</f>
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -1304,15 +1304,15 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -2576,11 +2576,15 @@
       <c r="D67" s="5">
         <v>5</v>
       </c>
-      <c r="E67" s="2"/>
-      <c r="F67" s="3"/>
+      <c r="E67" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G67" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
@@ -3154,7 +3158,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>